<commit_message>
falas do luke no primeiro filme
</commit_message>
<xml_diff>
--- a/SW - Episode IV.xlsx
+++ b/SW - Episode IV.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laris\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laris\Desktop\estudos_ferias20232\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A3242E-5F34-406A-B12C-413136621B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{06354364-EFD5-46B3-A85A-10C0CE3B6BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SW_EpisodeIV_ptBR" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="SW_EpisodeVI_ptBR" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -8241,7 +8242,7 @@
   </sheetPr>
   <dimension ref="A1:AI1011"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -26547,8 +26548,8 @@
   </sheetPr>
   <dimension ref="A1:H840"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>